<commit_message>
if en_Type2 ... end added, Line 255 to 271
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaoguowang/Documents/Developer/WorkSpace/Julia/playground/JuMP-Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF3EF96-9FC0-9143-A94A-FF0A47B6A538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3C6B6E-A748-0641-9D0F-01474E167783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2840" yWindow="5580" windowWidth="32300" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="6880" windowWidth="32300" windowHeight="9260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator Data" sheetId="1" r:id="rId1"/>
@@ -315,45 +315,45 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -361,7 +361,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -369,13 +369,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -383,13 +383,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1147,6 +1147,7 @@
     <cellStyle name="Followed Hyperlink 97" xfId="195" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
     <cellStyle name="Followed Hyperlink 98" xfId="197" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
     <cellStyle name="Followed Hyperlink 99" xfId="199" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink 10" xfId="20" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
     <cellStyle name="Hyperlink 100" xfId="200" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
     <cellStyle name="Hyperlink 101" xfId="202" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
@@ -1378,10 +1379,9 @@
     <cellStyle name="Hyperlink 97" xfId="194" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
     <cellStyle name="Hyperlink 98" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
     <cellStyle name="Hyperlink 99" xfId="198" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="适中" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1397,7 +1397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1719,11 +1719,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="6" bestFit="1" customWidth="1"/>
@@ -1752,7 +1752,7 @@
     <col min="25" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" ht="29.25" customHeight="1">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G4"/>
     </row>
   </sheetData>
@@ -1968,11 +1968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="5" width="14.1640625" customWidth="1"/>
@@ -1987,9 +1987,10 @@
     <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
     <col min="19" max="19" width="10.33203125" customWidth="1"/>
+    <col min="20" max="20" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="10" customFormat="1" ht="48" customHeight="1">
+    <row r="1" spans="1:21" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>72</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2184,7 +2185,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -2329,13 +2330,13 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="9.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="42.75" customHeight="1">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>7.6432569870451816</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>24.866368308677728</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2475,7 +2476,7 @@
         <v>0.25783100780887047</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>8.5943669269623477</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2586,10 +2587,10 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
@@ -2598,7 +2599,7 @@
     <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" ht="42.75" customHeight="1">
+    <row r="1" spans="1:9" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2656,7 +2657,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -2729,7 +2730,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
@@ -2740,7 +2741,7 @@
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.25" customHeight="1">
+    <row r="1" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>84</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F2" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
if en_Type3 ... end
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaoguowang/Documents/Developer/WorkSpace/Julia/playground/JuMP-Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3C6B6E-A748-0641-9D0F-01474E167783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B258056-A42E-3D48-887B-138513FFDAB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="6880" windowWidth="32300" windowHeight="9260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="6180" windowWidth="32300" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator Data" sheetId="1" r:id="rId1"/>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1889,6 +1889,15 @@
       <c r="T2" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="V2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -1952,6 +1961,15 @@
       </c>
       <c r="T3" s="6" t="s">
         <v>31</v>
+      </c>
+      <c r="V3" s="6">
+        <v>900</v>
+      </c>
+      <c r="W3" s="6">
+        <v>0</v>
+      </c>
+      <c r="X3" s="6">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1968,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add data for CsmDemand and PsmDemand
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaoguowang/Documents/Developer/WorkSpace/Julia/playground/JuMP-Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B258056-A42E-3D48-887B-138513FFDAB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07954B0D-8AFF-8A46-AB5D-5E62DE16FA93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="6180" windowWidth="32300" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10060" yWindow="8220" windowWidth="32300" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator Data" sheetId="1" r:id="rId1"/>
@@ -1720,7 +1720,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>